<commit_message>
add shops to joined data, convert metrics to 000
</commit_message>
<xml_diff>
--- a/codes/shop_order.xlsx
+++ b/codes/shop_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyzhur\Git\GP\PG_Clone\pg-dt-portal-for-nz\codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\d\Projects\!Projects\PG_portal\script\codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81ABE395-EA74-46E9-AEA2-39FEB081D0F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2153ADD-7BDB-4893-8CD6-B023C41A8FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6520" xr2:uid="{E07E7A11-EBB0-451D-A278-FEFCBE8D797A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E07E7A11-EBB0-451D-A278-FEFCBE8D797A}"/>
   </bookViews>
   <sheets>
     <sheet name="shop_order" sheetId="5" r:id="rId1"/>
@@ -27,12 +27,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="223">
   <si>
     <t>Value / Group name</t>
   </si>
@@ -590,9 +599,6 @@
   </si>
   <si>
     <t>5.1 Perekrestok</t>
-  </si>
-  <si>
-    <t>5.2 Perekryostok</t>
   </si>
   <si>
     <t>5.3 Atak</t>
@@ -710,7 +716,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,15 +751,8 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -778,6 +777,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -791,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -801,22 +806,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -832,9 +833,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -872,7 +873,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -978,7 +979,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1128,39 +1129,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7430144E-E3BF-44AA-B57B-6C6A3EF5D383}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.1796875" customWidth="1"/>
     <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="9"/>
-    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" style="16" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="16"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1172,10 +1172,10 @@
       <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="14">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1189,10 +1189,10 @@
       <c r="C3" s="17">
         <v>2</v>
       </c>
-      <c r="D3" s="14">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1206,10 +1206,10 @@
       <c r="C4" s="17">
         <v>3</v>
       </c>
-      <c r="D4" s="14">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1223,10 +1223,10 @@
       <c r="C5" s="17">
         <v>4</v>
       </c>
-      <c r="D5" s="14">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1240,10 +1240,10 @@
       <c r="C6" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="14">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1257,10 +1257,10 @@
       <c r="C7" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="14">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1274,10 +1274,10 @@
       <c r="C8" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="14">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1291,16 +1291,16 @@
       <c r="C9" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="14">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1308,10 +1308,10 @@
       <c r="C10" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="14">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1325,10 +1325,10 @@
       <c r="C11" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="14">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>183</v>
       </c>
     </row>
@@ -1342,10 +1342,10 @@
       <c r="C12" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="14">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>184</v>
       </c>
     </row>
@@ -1359,623 +1359,606 @@
       <c r="C13" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="14">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="14">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="14">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="14">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="14">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="14">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="14">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" s="14">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D22" s="14">
+        <v>147</v>
+      </c>
+      <c r="D22" s="1">
         <v>4</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="16" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="14">
+        <v>148</v>
+      </c>
+      <c r="D23" s="1">
         <v>4</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="16" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D24" s="14">
+        <v>149</v>
+      </c>
+      <c r="D24" s="1">
         <v>4</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="16" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="14">
-        <v>4</v>
-      </c>
-      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D26" s="14">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D27" s="14">
+        <v>152</v>
+      </c>
+      <c r="D27" s="1">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="16" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" s="14">
-        <v>4</v>
-      </c>
-      <c r="E28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" s="14">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="14">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="16" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="14">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="16" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="14">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="14">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D34" s="14">
-        <v>3</v>
-      </c>
-      <c r="E34" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D35" s="14">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3</v>
+      </c>
+      <c r="E35" s="16" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D36" s="14">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="D37" s="14">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
+      <c r="E37" s="16" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="D38" s="14">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="D39" s="14">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2</v>
+      </c>
+      <c r="E39" s="16" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D40" s="14">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="16" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D41" s="14">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s">
+        <v>166</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3</v>
+      </c>
+      <c r="E41" s="16" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D42" s="14">
-        <v>3</v>
-      </c>
-      <c r="E42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3</v>
+      </c>
+      <c r="E42" s="16" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" s="14">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
+        <v>168</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3</v>
+      </c>
+      <c r="E43" s="16" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="D44" s="14">
-        <v>3</v>
-      </c>
-      <c r="E44" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="16" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45" s="14">
-        <v>2</v>
-      </c>
-      <c r="E45" t="s">
+        <v>170</v>
+      </c>
+      <c r="D45" s="1">
+        <v>3</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D46" s="14">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3</v>
+      </c>
+      <c r="E46" s="16" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="D47" s="14">
-        <v>3</v>
-      </c>
-      <c r="E47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3</v>
+      </c>
+      <c r="E47" s="16" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="D48" s="14">
-        <v>3</v>
-      </c>
-      <c r="E48" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2</v>
+      </c>
+      <c r="E48" s="16" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49">
-        <v>48</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D49" s="14">
-        <v>2</v>
-      </c>
-      <c r="E49" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2047,7 +2030,7 @@
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
@@ -2079,7 +2062,7 @@
       <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
@@ -2111,7 +2094,7 @@
       <c r="E4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4">
         <v>3</v>
       </c>
       <c r="G4">
@@ -2143,7 +2126,7 @@
       <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5">
         <v>4</v>
       </c>
       <c r="G5">
@@ -2175,7 +2158,7 @@
       <c r="E6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6">
         <v>5</v>
       </c>
       <c r="G6">
@@ -2207,7 +2190,7 @@
       <c r="E7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7">
         <v>6</v>
       </c>
       <c r="G7">
@@ -2239,7 +2222,7 @@
       <c r="E8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8">
         <v>7</v>
       </c>
       <c r="G8" t="e">
@@ -2271,7 +2254,7 @@
       <c r="E9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9">
         <v>8</v>
       </c>
       <c r="G9">
@@ -2297,7 +2280,7 @@
       <c r="E10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" t="e">
@@ -2329,7 +2312,7 @@
       <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" t="e">
@@ -2355,7 +2338,7 @@
       <c r="E12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12">
         <v>11</v>
       </c>
       <c r="G12" t="e">
@@ -2381,7 +2364,7 @@
       <c r="E13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="e">
@@ -2410,7 +2393,7 @@
       <c r="E14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14">
         <v>13</v>
       </c>
       <c r="G14" t="e">
@@ -2439,7 +2422,7 @@
       <c r="E15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15">
         <v>14</v>
       </c>
       <c r="G15" t="e">
@@ -2465,7 +2448,7 @@
       <c r="E16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16">
         <v>15</v>
       </c>
       <c r="G16" t="e">
@@ -2494,7 +2477,7 @@
       <c r="E17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17">
         <v>16</v>
       </c>
       <c r="G17" t="e">
@@ -2520,7 +2503,7 @@
       <c r="E18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18">
         <v>17</v>
       </c>
       <c r="G18" t="e">
@@ -2546,7 +2529,7 @@
       <c r="E19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19">
         <v>18</v>
       </c>
       <c r="G19" t="e">
@@ -2572,7 +2555,7 @@
       <c r="E20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>19</v>
       </c>
       <c r="G20" t="e">
@@ -2598,7 +2581,7 @@
       <c r="E21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>20</v>
       </c>
       <c r="G21" t="e">
@@ -2624,7 +2607,7 @@
       <c r="E22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="e">
@@ -2650,7 +2633,7 @@
       <c r="E23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>22</v>
       </c>
       <c r="G23" t="e">
@@ -2676,7 +2659,7 @@
       <c r="E24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>23</v>
       </c>
       <c r="G24" t="e">
@@ -2702,7 +2685,7 @@
       <c r="E25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25">
         <v>24</v>
       </c>
       <c r="G25" t="e">
@@ -2728,7 +2711,7 @@
       <c r="E26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>25</v>
       </c>
       <c r="G26" t="e">
@@ -2754,7 +2737,7 @@
       <c r="E27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>26</v>
       </c>
       <c r="G27" t="e">
@@ -2780,7 +2763,7 @@
       <c r="E28" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>27</v>
       </c>
       <c r="G28" t="e">
@@ -2806,7 +2789,7 @@
       <c r="E29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29">
         <v>28</v>
       </c>
       <c r="G29" t="e">
@@ -2832,7 +2815,7 @@
       <c r="E30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30">
         <v>29</v>
       </c>
       <c r="G30" t="e">
@@ -2858,7 +2841,7 @@
       <c r="E31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31">
         <v>30</v>
       </c>
       <c r="G31" t="e">
@@ -2884,7 +2867,7 @@
       <c r="E32" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32">
         <v>31</v>
       </c>
       <c r="G32" t="e">
@@ -2910,7 +2893,7 @@
       <c r="E33" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33">
         <v>32</v>
       </c>
       <c r="G33" t="e">
@@ -2936,7 +2919,7 @@
       <c r="E34" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34">
         <v>33</v>
       </c>
       <c r="G34" t="e">
@@ -2962,7 +2945,7 @@
       <c r="E35" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35">
         <v>34</v>
       </c>
       <c r="G35" t="e">
@@ -2988,7 +2971,7 @@
       <c r="E36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36">
         <v>35</v>
       </c>
       <c r="G36" t="e">
@@ -3007,7 +2990,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+      <selection activeCell="G8" activeCellId="1" sqref="G10 G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3018,25 +3001,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3577,7 +3560,7 @@
       <c r="B25" s="4">
         <v>3</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>93</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -3646,7 +3629,7 @@
       <c r="B28" s="4">
         <v>2</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>96</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -3669,7 +3652,7 @@
       <c r="B29" s="4">
         <v>3</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
         <v>97</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -3692,7 +3675,7 @@
       <c r="B30" s="4">
         <v>3</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="11" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -3715,7 +3698,7 @@
       <c r="B31" s="4">
         <v>3</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -3761,7 +3744,7 @@
       <c r="B33" s="4">
         <v>3</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="11" t="s">
         <v>101</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -3784,7 +3767,7 @@
       <c r="B34" s="4">
         <v>3</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>102</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -3807,7 +3790,7 @@
       <c r="B35" s="4">
         <v>3</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="11" t="s">
         <v>103</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -3857,7 +3840,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+      <selection activeCell="G13" activeCellId="1" sqref="G10 G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3878,16 +3861,16 @@
       <c r="C1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4719,12 +4702,11 @@
     <col min="5" max="5" width="6.81640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="5.6328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="27.90625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="8.7265625" style="9"/>
     <col min="13" max="13" width="10.7265625" customWidth="1"/>
     <col min="14" max="14" width="20.08984375" customWidth="1"/>
     <col min="15" max="15" width="15.453125" customWidth="1"/>
     <col min="16" max="16" width="16.453125" customWidth="1"/>
-    <col min="17" max="17" width="15.6328125" style="17" customWidth="1"/>
+    <col min="17" max="17" width="15.6328125" style="14" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4741,22 +4723,22 @@
       <c r="D1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="9" t="s">
         <v>58</v>
       </c>
       <c r="M1" t="s">
@@ -4768,16 +4750,16 @@
       <c r="O1" t="s">
         <v>125</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="12" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4808,14 +4790,14 @@
         <f t="shared" ref="H2:H5" si="0">COUNTIF(J:J,G2)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="14">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="L2">
-        <f>COUNTIF(J:J,J2)</f>
+        <f t="shared" ref="L2:L16" si="1">COUNTIF(J:J,J2)</f>
         <v>1</v>
       </c>
       <c r="M2" t="str">
@@ -4832,10 +4814,10 @@
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" s="17">
-        <v>1</v>
-      </c>
-      <c r="R2" s="14">
+      <c r="Q2" s="14">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4850,7 +4832,7 @@
         <v>66</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D36" si="1">COUNTIF(J:J,C3)</f>
+        <f t="shared" ref="D3:D36" si="2">COUNTIF(J:J,C3)</f>
         <v>1</v>
       </c>
       <c r="E3" s="4">
@@ -4866,14 +4848,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I3" s="14">
-        <v>2</v>
-      </c>
-      <c r="J3" s="14" t="s">
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>66</v>
       </c>
       <c r="L3">
-        <f>COUNTIF(J:J,J3)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M3" t="str">
@@ -4890,10 +4872,10 @@
       <c r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" s="17">
-        <v>2</v>
-      </c>
-      <c r="R3" s="14">
+      <c r="Q3" s="14">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1">
         <v>2</v>
       </c>
     </row>
@@ -4908,7 +4890,7 @@
         <v>105</v>
       </c>
       <c r="D4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E4" s="4">
@@ -4924,14 +4906,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I4" s="14">
-        <v>2</v>
-      </c>
-      <c r="J4" s="14" t="s">
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>105</v>
       </c>
       <c r="L4">
-        <f>COUNTIF(J:J,J4)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M4" t="str">
@@ -4948,10 +4930,10 @@
       <c r="P4">
         <v>3</v>
       </c>
-      <c r="Q4" s="17">
-        <v>3</v>
-      </c>
-      <c r="R4" s="14">
+      <c r="Q4" s="14">
+        <v>3</v>
+      </c>
+      <c r="R4" s="1">
         <v>2</v>
       </c>
     </row>
@@ -4966,7 +4948,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E5" s="4">
@@ -4982,14 +4964,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I5" s="14">
-        <v>2</v>
-      </c>
-      <c r="J5" s="14" t="s">
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>69</v>
       </c>
       <c r="L5">
-        <f>COUNTIF(J:J,J5)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M5" t="str">
@@ -5006,10 +4988,10 @@
       <c r="P5">
         <v>4</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="Q5" s="14">
         <v>4</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5" s="1">
         <v>2</v>
       </c>
     </row>
@@ -5024,7 +5006,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E6" s="4">
@@ -5040,14 +5022,14 @@
         <f>COUNTIF(J:J,G6)</f>
         <v>1</v>
       </c>
-      <c r="I6" s="14">
-        <v>3</v>
-      </c>
-      <c r="J6" s="14" t="s">
+      <c r="I6" s="1">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>70</v>
       </c>
       <c r="L6">
-        <f>COUNTIF(J:J,J6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M6" t="str">
@@ -5064,10 +5046,10 @@
       <c r="P6">
         <v>5</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="Q6" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5082,7 +5064,7 @@
         <v>106</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E7" s="4">
@@ -5095,17 +5077,17 @@
         <v>73</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:H37" si="2">COUNTIF(J:J,G7)</f>
-        <v>1</v>
-      </c>
-      <c r="I7" s="14">
-        <v>3</v>
-      </c>
-      <c r="J7" s="14" t="s">
+        <f t="shared" ref="H7:H37" si="3">COUNTIF(J:J,G7)</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L7">
-        <f>COUNTIF(J:J,J7)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M7" t="str">
@@ -5122,10 +5104,10 @@
       <c r="P7">
         <v>6</v>
       </c>
-      <c r="Q7" s="17" t="s">
+      <c r="Q7" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5140,7 +5122,7 @@
         <v>107</v>
       </c>
       <c r="D8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E8" s="4">
@@ -5153,17 +5135,17 @@
         <v>74</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <v>3</v>
-      </c>
-      <c r="J8" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>107</v>
       </c>
       <c r="L8">
-        <f>COUNTIF(J:J,J8)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M8" t="str">
@@ -5180,10 +5162,10 @@
       <c r="P8">
         <v>7</v>
       </c>
-      <c r="Q8" s="17" t="s">
+      <c r="Q8" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5198,7 +5180,7 @@
         <v>73</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E9" s="4">
@@ -5211,17 +5193,17 @@
         <v>75</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I9" s="14">
-        <v>3</v>
-      </c>
-      <c r="J9" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>73</v>
       </c>
       <c r="L9">
-        <f>COUNTIF(J:J,J9)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M9" t="str">
@@ -5238,10 +5220,10 @@
       <c r="P9">
         <v>8</v>
       </c>
-      <c r="Q9" s="17" t="s">
+      <c r="Q9" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="R9" s="14">
+      <c r="R9" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5256,7 +5238,7 @@
         <v>108</v>
       </c>
       <c r="D10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E10" s="4">
@@ -5269,17 +5251,17 @@
         <v>76</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I10" s="14">
-        <v>3</v>
-      </c>
-      <c r="J10" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>108</v>
       </c>
       <c r="L10">
-        <f>COUNTIF(J:J,J10)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M10" t="str">
@@ -5296,10 +5278,10 @@
       <c r="P10">
         <v>9</v>
       </c>
-      <c r="Q10" s="17" t="s">
+      <c r="Q10" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="R10" s="14">
+      <c r="R10" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5314,7 +5296,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E11" s="4">
@@ -5327,17 +5309,17 @@
         <v>77</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I11" s="14">
-        <v>3</v>
-      </c>
-      <c r="J11" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>72</v>
       </c>
       <c r="L11">
-        <f>COUNTIF(J:J,J11)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M11" t="e">
@@ -5354,10 +5336,10 @@
       <c r="P11">
         <v>10</v>
       </c>
-      <c r="Q11" s="17" t="s">
+      <c r="Q11" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="R11" s="14">
+      <c r="R11" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5372,7 +5354,7 @@
         <v>109</v>
       </c>
       <c r="D12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E12" s="4">
@@ -5385,17 +5367,17 @@
         <v>78</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="14">
-        <v>2</v>
-      </c>
-      <c r="J12" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>75</v>
       </c>
       <c r="L12">
-        <f>COUNTIF(J:J,J12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M12" t="str">
@@ -5412,10 +5394,10 @@
       <c r="P12">
         <v>11</v>
       </c>
-      <c r="Q12" s="17" t="s">
+      <c r="Q12" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="R12" s="14">
+      <c r="R12" s="1">
         <v>2</v>
       </c>
     </row>
@@ -5430,7 +5412,7 @@
         <v>110</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E13" s="4">
@@ -5443,17 +5425,17 @@
         <v>79</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I13" s="14">
-        <v>3</v>
-      </c>
-      <c r="J13" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="L13">
-        <f>COUNTIF(J:J,J13)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M13" t="e">
@@ -5470,10 +5452,10 @@
       <c r="P13">
         <v>12</v>
       </c>
-      <c r="Q13" s="17" t="s">
+      <c r="Q13" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5488,7 +5470,7 @@
         <v>85</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E14" s="4">
@@ -5501,17 +5483,17 @@
         <v>80</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="14">
-        <v>3</v>
-      </c>
-      <c r="J14" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>110</v>
       </c>
       <c r="L14">
-        <f>COUNTIF(J:J,J14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M14" t="str">
@@ -5528,10 +5510,10 @@
       <c r="P14">
         <v>13</v>
       </c>
-      <c r="Q14" s="17" t="s">
+      <c r="Q14" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="R14" s="14">
+      <c r="R14" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5546,7 +5528,7 @@
         <v>77</v>
       </c>
       <c r="D15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E15" s="4">
@@ -5559,17 +5541,17 @@
         <v>81</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I15" s="14">
-        <v>3</v>
-      </c>
-      <c r="J15" s="14" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>109</v>
       </c>
       <c r="L15">
-        <f>COUNTIF(J:J,J15)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M15" t="str">
@@ -5586,10 +5568,10 @@
       <c r="P15">
         <v>14</v>
       </c>
-      <c r="Q15" s="17" t="s">
+      <c r="Q15" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="R15" s="14">
+      <c r="R15" s="1">
         <v>3</v>
       </c>
     </row>
@@ -5604,7 +5586,7 @@
         <v>78</v>
       </c>
       <c r="D16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E16" s="4">
@@ -5617,7 +5599,7 @@
         <v>82</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I16" s="7">
@@ -5627,7 +5609,7 @@
         <v>85</v>
       </c>
       <c r="L16">
-        <f>COUNTIF(J:J,J16)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M16" t="str">
@@ -5644,7 +5626,7 @@
       <c r="P16">
         <v>15</v>
       </c>
-      <c r="Q16" s="17" t="s">
+      <c r="Q16" s="14" t="s">
         <v>140</v>
       </c>
       <c r="R16" s="7">
@@ -5662,7 +5644,7 @@
         <v>79</v>
       </c>
       <c r="D17" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E17" s="4">
@@ -5675,7 +5657,7 @@
         <v>83</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I17" s="7">
@@ -5702,7 +5684,7 @@
       <c r="P17">
         <v>16</v>
       </c>
-      <c r="Q17" s="17" t="s">
+      <c r="Q17" s="14" t="s">
         <v>141</v>
       </c>
       <c r="R17" s="7">
@@ -5720,7 +5702,7 @@
         <v>80</v>
       </c>
       <c r="D18" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E18" s="4">
@@ -5733,7 +5715,7 @@
         <v>84</v>
       </c>
       <c r="H18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I18" s="7">
@@ -5756,7 +5738,7 @@
       <c r="P18">
         <v>17</v>
       </c>
-      <c r="Q18" s="17" t="s">
+      <c r="Q18" s="14" t="s">
         <v>142</v>
       </c>
       <c r="R18" s="7">
@@ -5774,7 +5756,7 @@
         <v>111</v>
       </c>
       <c r="D19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E19" s="4">
@@ -5787,7 +5769,7 @@
         <v>85</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I19" s="7">
@@ -5810,7 +5792,7 @@
       <c r="P19">
         <v>18</v>
       </c>
-      <c r="Q19" s="17" t="s">
+      <c r="Q19" s="14" t="s">
         <v>143</v>
       </c>
       <c r="R19" s="7">
@@ -5828,7 +5810,7 @@
         <v>81</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E20" s="4">
@@ -5841,7 +5823,7 @@
         <v>86</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I20" s="7">
@@ -5864,7 +5846,7 @@
       <c r="P20">
         <v>19</v>
       </c>
-      <c r="Q20" s="17" t="s">
+      <c r="Q20" s="14" t="s">
         <v>144</v>
       </c>
       <c r="R20" s="7">
@@ -5882,7 +5864,7 @@
         <v>82</v>
       </c>
       <c r="D21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E21" s="4">
@@ -5895,7 +5877,7 @@
         <v>87</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I21" s="4">
@@ -5918,7 +5900,7 @@
       <c r="P21">
         <v>20</v>
       </c>
-      <c r="Q21" s="17" t="s">
+      <c r="Q21" s="14" t="s">
         <v>145</v>
       </c>
       <c r="R21" s="4">
@@ -5936,7 +5918,7 @@
         <v>112</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E22" s="4">
@@ -5949,7 +5931,7 @@
         <v>88</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I22" s="4">
@@ -5972,7 +5954,7 @@
       <c r="P22">
         <v>21</v>
       </c>
-      <c r="Q22" s="17" t="s">
+      <c r="Q22" s="14" t="s">
         <v>146</v>
       </c>
       <c r="R22" s="4">
@@ -5990,7 +5972,7 @@
         <v>113</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E23" s="4">
@@ -6003,7 +5985,7 @@
         <v>91</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I23" s="4">
@@ -6026,7 +6008,7 @@
       <c r="P23">
         <v>22</v>
       </c>
-      <c r="Q23" s="17" t="s">
+      <c r="Q23" s="14" t="s">
         <v>147</v>
       </c>
       <c r="R23" s="4">
@@ -6044,7 +6026,7 @@
         <v>86</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E24" s="4">
@@ -6057,7 +6039,7 @@
         <v>92</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I24" s="4">
@@ -6080,7 +6062,7 @@
       <c r="P24">
         <v>23</v>
       </c>
-      <c r="Q24" s="17" t="s">
+      <c r="Q24" s="14" t="s">
         <v>148</v>
       </c>
       <c r="R24" s="4">
@@ -6098,7 +6080,7 @@
         <v>114</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E25" s="4">
@@ -6107,11 +6089,11 @@
       <c r="F25" s="4">
         <v>3</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="11" t="s">
         <v>93</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I25" s="7">
@@ -6134,7 +6116,7 @@
       <c r="P25">
         <v>24</v>
       </c>
-      <c r="Q25" s="17" t="s">
+      <c r="Q25" s="14" t="s">
         <v>149</v>
       </c>
       <c r="R25" s="7">
@@ -6152,7 +6134,7 @@
         <v>87</v>
       </c>
       <c r="D26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E26" s="4">
@@ -6165,7 +6147,7 @@
         <v>94</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I26" s="7">
@@ -6188,7 +6170,7 @@
       <c r="P26">
         <v>25</v>
       </c>
-      <c r="Q26" s="17" t="s">
+      <c r="Q26" s="14" t="s">
         <v>150</v>
       </c>
       <c r="R26" s="7">
@@ -6206,7 +6188,7 @@
         <v>115</v>
       </c>
       <c r="D27" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E27" s="4">
@@ -6219,7 +6201,7 @@
         <v>95</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I27" s="7">
@@ -6242,7 +6224,7 @@
       <c r="P27">
         <v>26</v>
       </c>
-      <c r="Q27" s="17" t="s">
+      <c r="Q27" s="14" t="s">
         <v>151</v>
       </c>
       <c r="R27" s="7">
@@ -6260,7 +6242,7 @@
         <v>91</v>
       </c>
       <c r="D28" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E28" s="4">
@@ -6269,11 +6251,11 @@
       <c r="F28" s="4">
         <v>2</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="11" t="s">
         <v>96</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I28" s="7">
@@ -6296,7 +6278,7 @@
       <c r="P28">
         <v>27</v>
       </c>
-      <c r="Q28" s="17" t="s">
+      <c r="Q28" s="14" t="s">
         <v>152</v>
       </c>
       <c r="R28" s="7">
@@ -6314,7 +6296,7 @@
         <v>92</v>
       </c>
       <c r="D29" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E29" s="4">
@@ -6323,11 +6305,11 @@
       <c r="F29" s="4">
         <v>3</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="11" t="s">
         <v>97</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I29" s="7">
@@ -6350,7 +6332,7 @@
       <c r="P29">
         <v>28</v>
       </c>
-      <c r="Q29" s="17" t="s">
+      <c r="Q29" s="14" t="s">
         <v>153</v>
       </c>
       <c r="R29" s="7">
@@ -6368,7 +6350,7 @@
         <v>117</v>
       </c>
       <c r="D30" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E30" s="4">
@@ -6377,11 +6359,11 @@
       <c r="F30" s="4">
         <v>3</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="11" t="s">
         <v>98</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I30" s="7">
@@ -6404,7 +6386,7 @@
       <c r="P30">
         <v>29</v>
       </c>
-      <c r="Q30" s="17" t="s">
+      <c r="Q30" s="14" t="s">
         <v>154</v>
       </c>
       <c r="R30" s="7">
@@ -6422,7 +6404,7 @@
         <v>94</v>
       </c>
       <c r="D31" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E31" s="4">
@@ -6431,11 +6413,11 @@
       <c r="F31" s="4">
         <v>3</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="11" t="s">
         <v>99</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I31" s="7">
@@ -6458,7 +6440,7 @@
       <c r="P31">
         <v>30</v>
       </c>
-      <c r="Q31" s="17" t="s">
+      <c r="Q31" s="14" t="s">
         <v>155</v>
       </c>
       <c r="R31" s="7">
@@ -6476,7 +6458,7 @@
         <v>118</v>
       </c>
       <c r="D32" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E32" s="4">
@@ -6489,7 +6471,7 @@
         <v>100</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I32" s="7">
@@ -6512,7 +6494,7 @@
       <c r="P32">
         <v>31</v>
       </c>
-      <c r="Q32" s="17" t="s">
+      <c r="Q32" s="14" t="s">
         <v>156</v>
       </c>
       <c r="R32" s="7">
@@ -6530,7 +6512,7 @@
         <v>83</v>
       </c>
       <c r="D33" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E33" s="4">
@@ -6539,11 +6521,11 @@
       <c r="F33" s="4">
         <v>3</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="11" t="s">
         <v>101</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I33" s="4">
@@ -6567,7 +6549,7 @@
       <c r="P33">
         <v>32</v>
       </c>
-      <c r="Q33" s="17" t="s">
+      <c r="Q33" s="14" t="s">
         <v>157</v>
       </c>
       <c r="R33" s="4">
@@ -6585,7 +6567,7 @@
         <v>119</v>
       </c>
       <c r="D34" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E34" s="4">
@@ -6594,11 +6576,11 @@
       <c r="F34" s="4">
         <v>3</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="11" t="s">
         <v>102</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I34" s="7">
@@ -6621,7 +6603,7 @@
       <c r="P34">
         <v>33</v>
       </c>
-      <c r="Q34" s="17" t="s">
+      <c r="Q34" s="14" t="s">
         <v>158</v>
       </c>
       <c r="R34" s="7">
@@ -6639,7 +6621,7 @@
         <v>100</v>
       </c>
       <c r="D35" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E35" s="4">
@@ -6648,11 +6630,11 @@
       <c r="F35" s="4">
         <v>3</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G35" s="11" t="s">
         <v>103</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I35" s="7">
@@ -6675,7 +6657,7 @@
       <c r="P35">
         <v>34</v>
       </c>
-      <c r="Q35" s="17" t="s">
+      <c r="Q35" s="14" t="s">
         <v>159</v>
       </c>
       <c r="R35" s="7">
@@ -6693,7 +6675,7 @@
         <v>120</v>
       </c>
       <c r="D36" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E36" s="4">
@@ -6706,7 +6688,7 @@
         <v>104</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I36" s="7">
@@ -6729,7 +6711,7 @@
       <c r="P36">
         <v>35</v>
       </c>
-      <c r="Q36" s="17" t="s">
+      <c r="Q36" s="14" t="s">
         <v>160</v>
       </c>
       <c r="R36" s="7">
@@ -6738,13 +6720,13 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I37" s="4">
         <v>3</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="J37" s="11" t="s">
         <v>93</v>
       </c>
       <c r="M37" t="e">
@@ -6761,7 +6743,7 @@
       <c r="P37">
         <v>36</v>
       </c>
-      <c r="Q37" s="17" t="s">
+      <c r="Q37" s="14" t="s">
         <v>161</v>
       </c>
       <c r="R37" s="4">
@@ -6789,7 +6771,7 @@
       <c r="P38">
         <v>37</v>
       </c>
-      <c r="Q38" s="17" t="s">
+      <c r="Q38" s="14" t="s">
         <v>162</v>
       </c>
       <c r="R38" s="7">
@@ -6817,7 +6799,7 @@
       <c r="P39">
         <v>38</v>
       </c>
-      <c r="Q39" s="17" t="s">
+      <c r="Q39" s="14" t="s">
         <v>163</v>
       </c>
       <c r="R39" s="4">
@@ -6845,7 +6827,7 @@
       <c r="P40">
         <v>39</v>
       </c>
-      <c r="Q40" s="17" t="s">
+      <c r="Q40" s="14" t="s">
         <v>164</v>
       </c>
       <c r="R40" s="7">
@@ -6856,7 +6838,7 @@
       <c r="I41" s="4">
         <v>2</v>
       </c>
-      <c r="J41" s="12" t="s">
+      <c r="J41" s="11" t="s">
         <v>96</v>
       </c>
       <c r="M41" t="e">
@@ -6873,7 +6855,7 @@
       <c r="P41">
         <v>40</v>
       </c>
-      <c r="Q41" s="17" t="s">
+      <c r="Q41" s="14" t="s">
         <v>165</v>
       </c>
       <c r="R41" s="4">
@@ -6884,7 +6866,7 @@
       <c r="I42" s="4">
         <v>3</v>
       </c>
-      <c r="J42" s="12" t="s">
+      <c r="J42" s="11" t="s">
         <v>97</v>
       </c>
       <c r="M42" t="e">
@@ -6901,7 +6883,7 @@
       <c r="P42">
         <v>41</v>
       </c>
-      <c r="Q42" s="17" t="s">
+      <c r="Q42" s="14" t="s">
         <v>166</v>
       </c>
       <c r="R42" s="4">
@@ -6912,7 +6894,7 @@
       <c r="I43" s="4">
         <v>3</v>
       </c>
-      <c r="J43" s="12" t="s">
+      <c r="J43" s="11" t="s">
         <v>98</v>
       </c>
       <c r="M43" t="e">
@@ -6929,7 +6911,7 @@
       <c r="P43">
         <v>42</v>
       </c>
-      <c r="Q43" s="17" t="s">
+      <c r="Q43" s="14" t="s">
         <v>167</v>
       </c>
       <c r="R43" s="4">
@@ -6940,7 +6922,7 @@
       <c r="I44" s="4">
         <v>3</v>
       </c>
-      <c r="J44" s="12" t="s">
+      <c r="J44" s="11" t="s">
         <v>99</v>
       </c>
       <c r="M44" t="e">
@@ -6957,7 +6939,7 @@
       <c r="P44">
         <v>43</v>
       </c>
-      <c r="Q44" s="17" t="s">
+      <c r="Q44" s="14" t="s">
         <v>168</v>
       </c>
       <c r="R44" s="4">
@@ -6985,7 +6967,7 @@
       <c r="P45">
         <v>44</v>
       </c>
-      <c r="Q45" s="17" t="s">
+      <c r="Q45" s="14" t="s">
         <v>169</v>
       </c>
       <c r="R45" s="4">
@@ -6996,7 +6978,7 @@
       <c r="I46" s="4">
         <v>3</v>
       </c>
-      <c r="J46" s="12" t="s">
+      <c r="J46" s="11" t="s">
         <v>101</v>
       </c>
       <c r="M46" t="e">
@@ -7013,7 +6995,7 @@
       <c r="P46">
         <v>45</v>
       </c>
-      <c r="Q46" s="17" t="s">
+      <c r="Q46" s="14" t="s">
         <v>170</v>
       </c>
       <c r="R46" s="4">
@@ -7024,7 +7006,7 @@
       <c r="I47" s="4">
         <v>3</v>
       </c>
-      <c r="J47" s="12" t="s">
+      <c r="J47" s="11" t="s">
         <v>102</v>
       </c>
       <c r="M47" t="e">
@@ -7041,7 +7023,7 @@
       <c r="P47">
         <v>46</v>
       </c>
-      <c r="Q47" s="17" t="s">
+      <c r="Q47" s="14" t="s">
         <v>171</v>
       </c>
       <c r="R47" s="4">
@@ -7052,7 +7034,7 @@
       <c r="I48" s="4">
         <v>3</v>
       </c>
-      <c r="J48" s="12" t="s">
+      <c r="J48" s="11" t="s">
         <v>103</v>
       </c>
       <c r="M48" t="e">
@@ -7069,7 +7051,7 @@
       <c r="P48">
         <v>47</v>
       </c>
-      <c r="Q48" s="17" t="s">
+      <c r="Q48" s="14" t="s">
         <v>172</v>
       </c>
       <c r="R48" s="4">
@@ -7097,7 +7079,7 @@
       <c r="P49">
         <v>48</v>
       </c>
-      <c r="Q49" s="17" t="s">
+      <c r="Q49" s="14" t="s">
         <v>173</v>
       </c>
       <c r="R49" s="4">

</xml_diff>

<commit_message>
add channel codes in excel
</commit_message>
<xml_diff>
--- a/codes/shop_order.xlsx
+++ b/codes/shop_order.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\d\Projects\!Projects\PG_portal\script\codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2153ADD-7BDB-4893-8CD6-B023C41A8FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E038FD3-903A-4020-9A99-66419E2D16D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E07E7A11-EBB0-451D-A278-FEFCBE8D797A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E07E7A11-EBB0-451D-A278-FEFCBE8D797A}"/>
   </bookViews>
   <sheets>
     <sheet name="shop_order" sheetId="5" r:id="rId1"/>
-    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
-    <sheet name="Подгузники" sheetId="2" r:id="rId3"/>
-    <sheet name="Остальное" sheetId="3" r:id="rId4"/>
-    <sheet name="Сведение осей" sheetId="4" r:id="rId5"/>
+    <sheet name="Иерархия от Натальи" sheetId="6" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId3"/>
+    <sheet name="Подгузники" sheetId="2" r:id="rId4"/>
+    <sheet name="Остальное" sheetId="3" r:id="rId5"/>
+    <sheet name="Сведение осей" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Сведение осей'!$A$1:$O$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">shop_order!$A$1:$H$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Сведение осей'!$A$1:$O$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="274">
   <si>
     <t>Value / Group name</t>
   </si>
@@ -565,63 +567,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>1 RUSSIA NATIONAL</t>
-  </si>
-  <si>
-    <t>2 Top Trade</t>
-  </si>
-  <si>
-    <t>3 All Hypermarket + Supermarket</t>
-  </si>
-  <si>
-    <t>4 All Hypermarket</t>
-  </si>
-  <si>
-    <t>4.1 Auchan</t>
-  </si>
-  <si>
-    <t>4.2 Karusel</t>
-  </si>
-  <si>
-    <t>4.3 Lenta Hyper</t>
-  </si>
-  <si>
-    <t>4.4 Magnit Hyper</t>
-  </si>
-  <si>
-    <t>4.5 Ok Hyper</t>
-  </si>
-  <si>
-    <t>4.6 Lenta</t>
-  </si>
-  <si>
-    <t>5 All Supermarket</t>
-  </si>
-  <si>
-    <t>5.1 Perekrestok</t>
-  </si>
-  <si>
-    <t>5.3 Atak</t>
-  </si>
-  <si>
-    <t>6 All HFS</t>
-  </si>
-  <si>
-    <t>7 All Cash &amp; Carry</t>
-  </si>
-  <si>
-    <t>7.1 Metro/Makro</t>
-  </si>
-  <si>
-    <t>7.2 Metro</t>
-  </si>
-  <si>
-    <t>8 All Discounter</t>
-  </si>
-  <si>
-    <t>8.1 Regular Discounter</t>
-  </si>
-  <si>
     <t>8.1.1 Dixy</t>
   </si>
   <si>
@@ -634,82 +579,292 @@
     <t>8.1.4 Monetka DSC</t>
   </si>
   <si>
-    <t>8.2 Hard Discounter</t>
-  </si>
-  <si>
     <t>8.2.1 Fix Price</t>
   </si>
   <si>
     <t>8.2.2 Svetofor</t>
   </si>
   <si>
-    <t>9 All Drug/Perfumery</t>
-  </si>
-  <si>
-    <t>10 All Perfumery</t>
-  </si>
-  <si>
-    <t>11 All Drug</t>
-  </si>
-  <si>
-    <t>12 All Drug chains</t>
-  </si>
-  <si>
-    <t>13 All Drug Chains</t>
-  </si>
-  <si>
-    <t>13.1 Magnit Cosmetic</t>
-  </si>
-  <si>
-    <t>13.2 Rubl Bum</t>
-  </si>
-  <si>
-    <t>13.3 Ulibka Radugi</t>
-  </si>
-  <si>
-    <t>13.4 Drug Chains wo Magnit and Rubl Bum</t>
-  </si>
-  <si>
-    <t>14 Independent Drugstores</t>
-  </si>
-  <si>
-    <t>15 All Chain Pharmacy/Independent Pharmacy</t>
-  </si>
-  <si>
-    <t>16 Pharmacy Total</t>
-  </si>
-  <si>
-    <t>17 Baby Store</t>
-  </si>
-  <si>
-    <t>17.1 Detskiy Mir</t>
-  </si>
-  <si>
-    <t>17.2 Korablic</t>
-  </si>
-  <si>
-    <t>17.3 Dochki-Synochki</t>
-  </si>
-  <si>
-    <t>18 All eCommerce</t>
-  </si>
-  <si>
-    <t>18.1 Detskiy Mir eCommerce</t>
-  </si>
-  <si>
-    <t>18.2 Ozon.ru</t>
-  </si>
-  <si>
-    <t>18.3 Wildberries.ru</t>
-  </si>
-  <si>
-    <t>19 All Other</t>
-  </si>
-  <si>
     <t>position_name_shop</t>
   </si>
   <si>
     <t>hier</t>
+  </si>
+  <si>
+    <t>Position Number all cat</t>
+  </si>
+  <si>
+    <t>Position Number Diapers</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Sub-channel</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Retailer</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>4.1.0</t>
+  </si>
+  <si>
+    <t>4.2.0</t>
+  </si>
+  <si>
+    <t>4.3.0</t>
+  </si>
+  <si>
+    <t>4.4.0</t>
+  </si>
+  <si>
+    <t>4.5.0</t>
+  </si>
+  <si>
+    <t>4.6.0</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>5.1.0</t>
+  </si>
+  <si>
+    <t>5.3.0</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
+  </si>
+  <si>
+    <t>7.0.0</t>
+  </si>
+  <si>
+    <t>7.1.0</t>
+  </si>
+  <si>
+    <t>7.2.0</t>
+  </si>
+  <si>
+    <t>8.0.0</t>
+  </si>
+  <si>
+    <t>8.1.0</t>
+  </si>
+  <si>
+    <t>8.2.0</t>
+  </si>
+  <si>
+    <t>9.0.0</t>
+  </si>
+  <si>
+    <t>10.0.0</t>
+  </si>
+  <si>
+    <t>11.0.0</t>
+  </si>
+  <si>
+    <t>12.0.0</t>
+  </si>
+  <si>
+    <t>13.0.0</t>
+  </si>
+  <si>
+    <t>13.1.0</t>
+  </si>
+  <si>
+    <t>13.2.0</t>
+  </si>
+  <si>
+    <t>13.3.0</t>
+  </si>
+  <si>
+    <t>13.4.0</t>
+  </si>
+  <si>
+    <t>14.0.0</t>
+  </si>
+  <si>
+    <t>15.0.0</t>
+  </si>
+  <si>
+    <t>16.0.0</t>
+  </si>
+  <si>
+    <t>17.0.0</t>
+  </si>
+  <si>
+    <t>17.1.0</t>
+  </si>
+  <si>
+    <t>17.2.0</t>
+  </si>
+  <si>
+    <t>17.3.0</t>
+  </si>
+  <si>
+    <t>18.0.0</t>
+  </si>
+  <si>
+    <t>18.1.0</t>
+  </si>
+  <si>
+    <t>18.2.0</t>
+  </si>
+  <si>
+    <t>18.3.0</t>
+  </si>
+  <si>
+    <t>19.0.0</t>
+  </si>
+  <si>
+    <t>1.0.0 RUSSIA NATIONAL</t>
+  </si>
+  <si>
+    <t>2.0.0 Top Trade</t>
+  </si>
+  <si>
+    <t>3.0.0 All Hypermarket + Supermarket</t>
+  </si>
+  <si>
+    <t>4.0.0 All Hypermarket</t>
+  </si>
+  <si>
+    <t>4.1.0 Auchan</t>
+  </si>
+  <si>
+    <t>4.2.0 Karusel</t>
+  </si>
+  <si>
+    <t>4.3.0 Lenta Hyper</t>
+  </si>
+  <si>
+    <t>4.4.0 Magnit Hyper</t>
+  </si>
+  <si>
+    <t>4.5.0 Ok Hyper</t>
+  </si>
+  <si>
+    <t>4.6.0 Lenta</t>
+  </si>
+  <si>
+    <t>5.0.0 All Supermarket</t>
+  </si>
+  <si>
+    <t>5.1.0 Perekrestok</t>
+  </si>
+  <si>
+    <t>5.3.0 Atak</t>
+  </si>
+  <si>
+    <t>6.0.0 All HFS</t>
+  </si>
+  <si>
+    <t>7.0.0 All Cash &amp; Carry</t>
+  </si>
+  <si>
+    <t>7.1.0 Metro/Makro</t>
+  </si>
+  <si>
+    <t>7.2.0 Metro</t>
+  </si>
+  <si>
+    <t>8.0.0 All Discounter</t>
+  </si>
+  <si>
+    <t>8.1.0 Regular Discounter</t>
+  </si>
+  <si>
+    <t>8.2.0 Hard Discounter</t>
+  </si>
+  <si>
+    <t>9.0.0 All Drug/Perfumery</t>
+  </si>
+  <si>
+    <t>10.0.0 All Perfumery</t>
+  </si>
+  <si>
+    <t>11.0.0 All Drug</t>
+  </si>
+  <si>
+    <t>12.0.0 All Drug chains</t>
+  </si>
+  <si>
+    <t>13.0.0 All Drug Chains</t>
+  </si>
+  <si>
+    <t>13.1.0 Magnit Cosmetic</t>
+  </si>
+  <si>
+    <t>13.2.0 Rubl Bum</t>
+  </si>
+  <si>
+    <t>13.3.0 Ulibka Radugi</t>
+  </si>
+  <si>
+    <t>13.4.0 Drug Chains wo Magnit and Rubl Bum</t>
+  </si>
+  <si>
+    <t>14.0.0 Independent Drugstores</t>
+  </si>
+  <si>
+    <t>15.0.0 All Chain Pharmacy/Independent Pharmacy</t>
+  </si>
+  <si>
+    <t>16.0.0 Pharmacy Total</t>
+  </si>
+  <si>
+    <t>17.0.0 Baby Store</t>
+  </si>
+  <si>
+    <t>17.1.0 Detskiy Mir</t>
+  </si>
+  <si>
+    <t>17.2.0 Korablic</t>
+  </si>
+  <si>
+    <t>17.3.0 Dochki-Synochki</t>
+  </si>
+  <si>
+    <t>18.0.0 All eCommerce</t>
+  </si>
+  <si>
+    <t>18.1.0 Detskiy Mir eCommerce</t>
+  </si>
+  <si>
+    <t>18.2.0 Ozon.ru</t>
+  </si>
+  <si>
+    <t>18.3.0 Wildberries.ru</t>
+  </si>
+  <si>
+    <t>19.0.0 All Other</t>
+  </si>
+  <si>
+    <t>shop_name</t>
+  </si>
+  <si>
+    <t>channel_type</t>
+  </si>
+  <si>
+    <t>channel_code</t>
   </si>
 </sst>
 </file>
@@ -752,7 +907,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,6 +938,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -796,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -815,6 +976,9 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7430144E-E3BF-44AA-B57B-6C6A3EF5D383}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1140,19 +1304,21 @@
     <col min="1" max="1" width="23.1796875" customWidth="1"/>
     <col min="2" max="2" width="20.6328125" customWidth="1"/>
     <col min="3" max="3" width="10.453125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="29.1796875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="5" max="5" width="34" style="16" customWidth="1"/>
+    <col min="6" max="6" width="21.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="2"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>126</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>222</v>
+        <v>181</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>129</v>
@@ -1160,77 +1326,121 @@
       <c r="E1" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F1" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="17">
-        <v>1</v>
+      <c r="C2" s="17" t="s">
+        <v>189</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="17">
-        <v>2</v>
+      <c r="C3" s="17" t="s">
+        <v>190</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>231</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="17">
-        <v>3</v>
+      <c r="C4" s="17" t="s">
+        <v>191</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>232</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="17">
-        <v>4</v>
+      <c r="C5" s="17" t="s">
+        <v>192</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1238,16 +1448,25 @@
         <v>5</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1255,16 +1474,25 @@
         <v>6</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1272,16 +1500,25 @@
         <v>7</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1289,16 +1526,25 @@
         <v>8</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>133</v>
+        <v>196</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1306,16 +1552,25 @@
         <v>9</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>134</v>
+        <v>197</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1323,16 +1578,25 @@
         <v>10</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>135</v>
+        <v>198</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" s="2">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1340,16 +1604,25 @@
         <v>11</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>136</v>
+        <v>199</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1357,16 +1630,25 @@
         <v>12</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G13" s="2">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1374,16 +1656,25 @@
         <v>13</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>139</v>
+        <v>201</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>242</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1391,16 +1682,25 @@
         <v>14</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1408,16 +1708,25 @@
         <v>15</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>141</v>
+        <v>203</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1425,16 +1734,25 @@
         <v>16</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="D17" s="1">
         <v>3</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="2">
+        <v>4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1442,16 +1760,25 @@
         <v>17</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1459,16 +1786,25 @@
         <v>18</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1476,16 +1812,25 @@
         <v>19</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>145</v>
+        <v>207</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1499,10 +1844,19 @@
         <v>4</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G21" s="2">
+        <v>4</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1516,10 +1870,19 @@
         <v>4</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G22" s="2">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1533,10 +1896,19 @@
         <v>4</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G23" s="2">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1550,10 +1922,19 @@
         <v>4</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G24" s="2">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1561,16 +1942,25 @@
         <v>24</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="2">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1584,10 +1974,19 @@
         <v>4</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" s="2">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1601,10 +2000,19 @@
         <v>4</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1612,16 +2020,25 @@
         <v>27</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>153</v>
+        <v>209</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1629,16 +2046,25 @@
         <v>28</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>154</v>
+        <v>210</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G29" s="2">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1646,16 +2072,25 @@
         <v>29</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>155</v>
+        <v>211</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1663,16 +2098,25 @@
         <v>30</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>156</v>
+        <v>212</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+        <v>253</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G31" s="2">
+        <v>3</v>
+      </c>
+      <c r="H31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1680,16 +2124,25 @@
         <v>31</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="D32" s="1">
         <v>2</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1697,16 +2150,25 @@
         <v>32</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>158</v>
+        <v>214</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G33" s="2">
+        <v>4</v>
+      </c>
+      <c r="H33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1714,16 +2176,25 @@
         <v>33</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" s="2">
+        <v>4</v>
+      </c>
+      <c r="H34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1731,16 +2202,25 @@
         <v>34</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G35" s="2">
+        <v>4</v>
+      </c>
+      <c r="H35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1748,16 +2228,25 @@
         <v>35</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G36" s="2">
+        <v>4</v>
+      </c>
+      <c r="H36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1765,16 +2254,25 @@
         <v>36</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="D37" s="1">
         <v>2</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G37" s="2">
+        <v>3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1782,16 +2280,25 @@
         <v>37</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="D38" s="1">
         <v>2</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G38" s="2">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1799,16 +2306,25 @@
         <v>38</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="D39" s="1">
         <v>2</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="2">
+        <v>2</v>
+      </c>
+      <c r="H39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -1816,16 +2332,25 @@
         <v>39</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>165</v>
+        <v>221</v>
       </c>
       <c r="D40" s="1">
         <v>2</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>262</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G40" s="2">
+        <v>2</v>
+      </c>
+      <c r="H40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -1833,16 +2358,25 @@
         <v>40</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G41" s="2">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -1850,16 +2384,25 @@
         <v>41</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>167</v>
+        <v>223</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G42" s="2">
+        <v>4</v>
+      </c>
+      <c r="H42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -1867,16 +2410,25 @@
         <v>42</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="2">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1884,16 +2436,25 @@
         <v>43</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>169</v>
+        <v>225</v>
       </c>
       <c r="D44" s="1">
         <v>2</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G44" s="2">
+        <v>2</v>
+      </c>
+      <c r="H44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -1901,16 +2462,25 @@
         <v>44</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G45" s="2">
+        <v>4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1918,16 +2488,25 @@
         <v>45</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="D46" s="1">
         <v>3</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G46" s="2">
+        <v>4</v>
+      </c>
+      <c r="H46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1935,16 +2514,25 @@
         <v>46</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>172</v>
+        <v>228</v>
       </c>
       <c r="D47" s="1">
         <v>3</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G47" s="2">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -1952,13 +2540,982 @@
         <v>47</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>173</v>
+        <v>229</v>
       </c>
       <c r="D48" s="1">
         <v>2</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>220</v>
+        <v>270</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G48" s="2">
+        <v>2</v>
+      </c>
+      <c r="H48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H48" xr:uid="{11575B49-7BD6-46F6-8AD7-2C062E9EFCE0}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FD7414-398E-422F-B728-74C11128479D}">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="1">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="1">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F14" s="1">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="1">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F16" s="1">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="1">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="1">
+        <v>17</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="1">
+        <v>18</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="1">
+        <v>19</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="1">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="1">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="1">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F24" s="1">
+        <v>23</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F25" s="1">
+        <v>24</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F26" s="1">
+        <v>25</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F27" s="1">
+        <v>26</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F28" s="1">
+        <v>27</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" s="1">
+        <v>28</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" s="1">
+        <v>29</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="1">
+        <v>30</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F32" s="1">
+        <v>31</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33" s="1">
+        <v>32</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F34" s="1">
+        <v>33</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F35" s="1">
+        <v>34</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F36" s="1">
+        <v>35</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1966,7 +3523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B8EA30-0557-4519-8B35-1DA7FB5134F4}">
   <dimension ref="A1:I36"/>
   <sheetViews>
@@ -2985,12 +4542,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809DCA4E-8E2F-47A2-B53F-15BD1F8E281A}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" activeCellId="1" sqref="G10 G8"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3000,7 +4557,7 @@
     <col min="4" max="4" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -3023,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3045,8 +4602,9 @@
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3068,8 +4626,9 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3091,8 +4650,9 @@
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3114,8 +4674,9 @@
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3137,8 +4698,9 @@
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3160,8 +4722,9 @@
       <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3183,8 +4746,9 @@
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3206,8 +4770,9 @@
       <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3230,8 +4795,9 @@
         <v>9</v>
       </c>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3253,8 +4819,9 @@
       <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3276,8 +4843,9 @@
       <c r="G12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3299,8 +4867,9 @@
       <c r="G13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3322,8 +4891,9 @@
       <c r="G14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3345,8 +4915,9 @@
       <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3368,8 +4939,9 @@
       <c r="G16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3391,8 +4963,9 @@
       <c r="G17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3414,8 +4987,9 @@
       <c r="G18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3437,8 +5011,9 @@
       <c r="G19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3460,8 +5035,9 @@
       <c r="G20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3483,8 +5059,9 @@
       <c r="G21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3506,8 +5083,9 @@
       <c r="G22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3529,8 +5107,9 @@
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3552,8 +5131,9 @@
       <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3575,8 +5155,9 @@
       <c r="G25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3598,8 +5179,9 @@
       <c r="G26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3621,8 +5203,9 @@
       <c r="G27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -3644,8 +5227,9 @@
       <c r="G28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3667,8 +5251,9 @@
       <c r="G29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3690,8 +5275,9 @@
       <c r="G30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -3713,8 +5299,9 @@
       <c r="G31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I31" s="19"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3736,8 +5323,9 @@
       <c r="G32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3759,8 +5347,9 @@
       <c r="G33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I33" s="19"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -3782,8 +5371,9 @@
       <c r="G34" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I34" s="19"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3805,8 +5395,9 @@
       <c r="G35" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I35" s="19"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3828,6 +5419,7 @@
       <c r="G36" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="I36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3835,12 +5427,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B29EBE5-C1FB-4F9A-B77F-3C27D9C13D75}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" activeCellId="1" sqref="G10 G13"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3851,7 +5443,7 @@
     <col min="6" max="6" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>56</v>
       </c>
@@ -3874,7 +5466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -3896,8 +5488,11 @@
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -3919,8 +5514,11 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -3942,8 +5540,11 @@
       <c r="G4" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -3965,8 +5566,11 @@
       <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -3988,8 +5592,11 @@
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -4011,8 +5618,11 @@
       <c r="G7" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I7" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -4034,8 +5644,11 @@
       <c r="G8" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I8" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -4057,8 +5670,11 @@
       <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I9" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -4080,8 +5696,11 @@
       <c r="G10" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I10" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -4103,8 +5722,11 @@
       <c r="G11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -4126,8 +5748,11 @@
       <c r="G12" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I12" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -4149,8 +5774,11 @@
       <c r="G13" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -4172,8 +5800,11 @@
       <c r="G14" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I14" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -4195,8 +5826,11 @@
       <c r="G15" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -4218,8 +5852,11 @@
       <c r="G16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -4241,8 +5878,11 @@
       <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -4264,8 +5904,11 @@
       <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -4287,8 +5930,11 @@
       <c r="G19" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I19" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -4310,8 +5956,11 @@
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I20" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -4333,8 +5982,11 @@
       <c r="G21" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I21" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -4356,8 +6008,11 @@
       <c r="G22" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I22" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -4379,8 +6034,11 @@
       <c r="G23" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I23" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -4402,8 +6060,11 @@
       <c r="G24" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I24" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -4425,8 +6086,11 @@
       <c r="G25" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I25" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -4448,8 +6112,11 @@
       <c r="G26" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I26" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -4471,8 +6138,11 @@
       <c r="G27" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I27" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -4494,8 +6164,11 @@
       <c r="G28" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -4517,8 +6190,11 @@
       <c r="G29" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -4540,8 +6216,11 @@
       <c r="G30" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I30" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -4563,8 +6242,11 @@
       <c r="G31" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I31" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -4586,8 +6268,11 @@
       <c r="G32" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I32" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -4609,8 +6294,11 @@
       <c r="G33" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I33" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -4632,8 +6320,11 @@
       <c r="G34" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I34" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -4655,8 +6346,11 @@
       <c r="G35" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -4677,6 +6371,9 @@
       </c>
       <c r="G36" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4685,12 +6382,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E7458B-240E-4361-B7F0-A2BA12AD8F30}">
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>